<commit_message>
Particles.js background en login fixes
</commit_message>
<xml_diff>
--- a/files/Test1234/converted/Bestand1.xlsx
+++ b/files/Test1234/converted/Bestand1.xlsx
@@ -348,7 +348,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Data bestand 1Dit is bestand 2 column 2Dit is bestand 2 column 2Dit is bestand 2 column 2</t>
+          <t>Data bestand 1</t>
         </is>
       </c>
     </row>
@@ -365,7 +365,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dwadwaBestand 2 column 7Bestand 2 column 7Bestand 2 column 7</t>
+          <t>dwadwaadaB</t>
         </is>
       </c>
     </row>
@@ -399,7 +399,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dadaBestand 2 column 4Bestand 2 column 4Bestand 2 column 4</t>
+          <t>dadadwadwaAB</t>
         </is>
       </c>
     </row>
@@ -433,7 +433,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dadaBestand 2 column 6Bestand 2 column 6Bestand 2 column 6</t>
+          <t>dadadadaB</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>asdBestand 2 column 9Bestand 2 column 9Bestand 2 column 9</t>
+          <t>asddadaB</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>wasdwaBestand 2 column 8Bestand 2 column 12Bestand 2 column 8Bestand 2 column 12Bestand 2 column 8Bestand 2 column 12</t>
+          <t>wasdwaB</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dwadwaBestand 2 column 11Bestand 2 column 11Bestand 2 column 11</t>
+          <t>dwadwadadaB</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sdwaBestand 2 column 10Bestand 2 column 10Bestand 2 column 10</t>
+          <t>sdwadadaB</t>
         </is>
       </c>
     </row>

</xml_diff>